<commit_message>
updated slots on oscem_* schemas
</commit_message>
<xml_diff>
--- a/project/excel/oscem_schemas.xlsx
+++ b/project/excel/oscem_schemas.xlsx
@@ -1,36 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TiltAngle" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Any" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Range" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Series" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="ImageSize" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="BoundingBox2D" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="QuantityValue" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Acquisition" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="EnergyFilter" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="SpecialistOptics" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Phaseplate" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="SphericalAberrationCorrector" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="ChromaticAberrationCorrector" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Instrument" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Person" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Author" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Grant" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="OverallMolecule" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="Molecule" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="Ligand" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="Specimen" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="Grid" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="Sample" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="EMDataset" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TiltAngle" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Any" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Range" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Series" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ImageSize" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BoundingBox2D" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QuantityValue" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Acquisition" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EnergyFilter" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecialistOptics" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Phaseplate" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SphericalAberrationCorrector" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChromaticAberrationCorrector" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instrument" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Person" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Author" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grant" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OverallMolecule" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Molecule" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ligand" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Specimen" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grid" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sample" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EMDataset" sheetId="24" state="visible" r:id="rId24"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -835,7 +835,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -864,8 +864,18 @@
           <t>molecular_weight</t>
         </is>
       </c>
-    </row>
-  </sheetData>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>assembly</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"FILAMENT,HELICAL ARRAY,PARTICLE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated descriptor to allow "Any"
</commit_message>
<xml_diff>
--- a/project/excel/oscem_schemas.xlsx
+++ b/project/excel/oscem_schemas.xlsx
@@ -14,23 +14,38 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ImageSize" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BoundingBox2D" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QuantityValue" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Acquisition" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EnergyFilter" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecialistOptics" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Phaseplate" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SphericalAberrationCorrector" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChromaticAberrationCorrector" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instrument" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Person" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Author" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grant" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OverallMolecule" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Molecule" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ligand" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Specimen" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grid" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sample" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EMDataset" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Descriptors" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Acquisition" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EnergyFilter" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecialistOptics" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Phaseplate" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SphericalAberrationCorrector" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChromaticAberrationCorrector" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instrument" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Person" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Author" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grant" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OverallMolecule" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Molecule" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ligand" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Specimen" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grid" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sample" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Movies" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Micrographs" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CTFs" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Defocus" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Resolution" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Astigmatism" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Coordinates" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Classes2D" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Classes3D" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Volume" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OrthogonalSlices" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IsosurfaceImages" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Volumes" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Processing" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EMDataset" sheetId="39" state="visible" r:id="rId39"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -483,6 +498,42 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>used</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>model</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>width</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>phaseplate</t>
         </is>
       </c>
@@ -502,7 +553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -533,7 +584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -564,7 +615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -595,7 +646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -651,7 +702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -697,7 +748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -773,7 +824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -829,7 +880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -880,7 +931,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -951,7 +1020,477 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>present</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>smiles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>reference</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>buffer</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>concentration</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ph</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>vitrification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>vitrification_cryogen</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>humidity</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>temperature</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>staining</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>embedding</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>shadowing</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>material</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>mesh</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>film_support</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>film_material</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>film_topology</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>film_thickness</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>pretreatment_type</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>pretreatment_time</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>pretreatment_pressure</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>pretreatment_atmosphere</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>overall_molecule</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>molecule</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ligands</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>specimen</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>grid</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dose_per_image</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>initial_dose</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>gain_image</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>dark_image</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>descriptors</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>number_micrographs</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>descriptors</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>amplitude_contrast</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>defocus</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>resolution</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>astigmatism</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>descriptors</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>output_min_defocus</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output_max_defocus</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_avg_defocus</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>defocus_histogram</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>defocus_micrograph_examples</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>output_min_resolution</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>output_max_resolution</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>output_avg_resolution</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>resolution_histogram</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>maximal</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -964,12 +1503,199 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>astigmatism_histogram</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>number_particles</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>particles_per_micrograph</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>num_source_micrographs</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>particles_histogram</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>micrograph_examples</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>descriptors</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>number_classes_2D</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>particles_per_2Dclass</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>images_classes_2D</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>resolution_classes_2D</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>descriptors</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>number_classes_3D</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>particles_per_3Dclass</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>images_classes_3D</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>volume</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>resolution_classes_3D</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>descriptors</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>orthogonal_slices</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>isosurface_images</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -986,501 +1712,461 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>present</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>smiles</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>reference</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>buffer</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>concentration</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ph</t>
+          <t>orthogonal_slices_X</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>orthogonal_slices_Y</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>orthogonal_slices_Z</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>front_view</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>side_view</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>top_view</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>volume_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>vol_number_particles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>size</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>vitrification</t>
+          <t>orthogonal_slices</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>vitrification_cryogen</t>
+          <t>isosurface_images</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>humidity</t>
+          <t>vol_resolution</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>temperature</t>
+          <t>descriptors</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>movies</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>micrographs</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ctfs</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>coordinates</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>classes2D</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>classes3D</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>volumes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>acquisition</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>instrument</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>grants</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>authors</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>processing</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>increment</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>maximal</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>height</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>width</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>x_min</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>x_max</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>y_min</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>y_max</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>descriptor_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>descriptor_thing</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AA1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>nominal_defocus</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>calibrated_defocus</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nominal_magnification</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>calibrated_magnification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>holder</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>holder_cryogen</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>temperature_range</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>staining</t>
+          <t>microscope_software</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>embedding</t>
+          <t>detector</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>shadowing</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>material</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>mesh</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>film_support</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>film_material</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>film_topology</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>film_thickness</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>pretreatment_type</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>pretreatment_time</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>pretreatment_pressure</t>
+          <t>detector_mode</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>pretreatment_atmosphere</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>overall_molecule</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>molecule</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>ligands</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>specimen</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>grid</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>acquisition</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>instrument</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>sample</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>grants</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>authors</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>minimal</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>maximal</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>increment</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>minimal</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>maximal</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>height</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>width</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>x_min</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>x_max</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>y_min</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>y_max</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AA1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>nominal_defocus</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>calibrated_defocus</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nominal_magnification</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>calibrated_magnification</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>holder</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>holder_cryogen</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>temperature_range</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>microscope_software</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>detector</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>detector_mode</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
           <t>dose_per_movie</t>
         </is>
       </c>
@@ -1568,40 +2254,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>used</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>model</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>width</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>